<commit_message>
cambios en las preguntas
</commit_message>
<xml_diff>
--- a/cuadro_de_recomendacion.xlsx
+++ b/cuadro_de_recomendacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frusc\Desktop\5to CICLO - D.E.G\LP3-Danilo\Trabajo\Experto_prueba_estadistica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{17C7EAF5-F635-43AF-AC70-AC2F3C5539F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5BBEF8-BE06-4DF4-9CC0-AE94606AE5E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20690" yWindow="122" windowWidth="13856" windowHeight="18544" xr2:uid="{A7589141-8C65-4603-9469-2ACC79CE9FA5}"/>
+    <workbookView xWindow="20581" yWindow="163" windowWidth="13857" windowHeight="18543" xr2:uid="{A7589141-8C65-4603-9469-2ACC79CE9FA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -608,7 +608,7 @@
   <dimension ref="B2:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A4" sqref="A3:A4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>

</xml_diff>